<commit_message>
Organisational practices loading (not to use)
</commit_message>
<xml_diff>
--- a/Results/org_practices_loadings.xlsx
+++ b/Results/org_practices_loadings.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="45">
   <si>
     <t>lhs</t>
   </si>
@@ -107,16 +107,19 @@
     <t>20</t>
   </si>
   <si>
+    <t>21</t>
+  </si>
+  <si>
     <t>organisational_practices</t>
   </si>
   <si>
-    <t>Q300</t>
-  </si>
-  <si>
-    <t>Q301</t>
-  </si>
-  <si>
-    <t>Q302</t>
+    <t>practice_stress</t>
+  </si>
+  <si>
+    <t>practice_harassment</t>
+  </si>
+  <si>
+    <t>practice_violence</t>
   </si>
   <si>
     <t>=~</t>
@@ -138,6 +141,9 @@
   </si>
   <si>
     <t>t1</t>
+  </si>
+  <si>
+    <t>t2</t>
   </si>
   <si>
     <t/>
@@ -232,13 +238,13 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" t="n">
         <v>0.0</v>
@@ -256,13 +262,13 @@
         <v>#N/A</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6018040122255537</v>
+        <v>0.6002659287377311</v>
       </c>
       <c r="K2" t="n">
-        <v>0.6018040122255537</v>
+        <v>0.6002659287377311</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6018040122255537</v>
+        <v>0.6002659287377311</v>
       </c>
     </row>
     <row r="3">
@@ -270,37 +276,37 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" t="n">
         <v>0.0</v>
       </c>
       <c r="F3" t="n">
-        <v>1.5371373762778846</v>
+        <v>1.543217570976869</v>
       </c>
       <c r="G3" t="n">
-        <v>0.03282002010493717</v>
+        <v>0.03317370897430347</v>
       </c>
       <c r="H3" t="n">
-        <v>46.83535754588556</v>
+        <v>46.51929551116077</v>
       </c>
       <c r="I3" t="n">
         <v>0.0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9250554403858916</v>
+        <v>0.9263409284868157</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9250554403858916</v>
+        <v>0.9263409284868157</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9250554403858916</v>
+        <v>0.9263409284868157</v>
       </c>
     </row>
     <row r="4">
@@ -308,37 +314,37 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
       <c r="E4" t="n">
         <v>0.0</v>
       </c>
       <c r="F4" t="n">
-        <v>1.3885953265469624</v>
+        <v>1.3791082610333982</v>
       </c>
       <c r="G4" t="n">
-        <v>0.026614619696304707</v>
+        <v>0.026418527188628395</v>
       </c>
       <c r="H4" t="n">
-        <v>52.1741562491596</v>
+        <v>52.20231435259655</v>
       </c>
       <c r="I4" t="n">
         <v>0.0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8356622388736149</v>
+        <v>0.8278317011390901</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8356622388736149</v>
+        <v>0.8278317011390901</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8356622388736149</v>
+        <v>0.8278317011390901</v>
       </c>
     </row>
     <row r="5">
@@ -346,37 +352,37 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E5" t="n">
         <v>0.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.33120888275116667</v>
+        <v>0.33008541681176606</v>
       </c>
       <c r="G5" t="n">
-        <v>0.010384292933147878</v>
+        <v>0.010329200041895775</v>
       </c>
       <c r="H5" t="n">
-        <v>31.895179082815467</v>
+        <v>31.956532497475347</v>
       </c>
       <c r="I5" t="n">
         <v>0.0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.33120888275116667</v>
+        <v>0.33008541681176606</v>
       </c>
       <c r="K5" t="n">
-        <v>0.33120888275116667</v>
+        <v>0.33008541681176606</v>
       </c>
       <c r="L5" t="n">
-        <v>0.33120888275116667</v>
+        <v>0.33008541681176606</v>
       </c>
     </row>
     <row r="6">
@@ -384,37 +390,37 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E6" t="n">
         <v>0.0</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.17336780553058911</v>
+        <v>-0.17588065544773837</v>
       </c>
       <c r="G6" t="n">
-        <v>0.010234568753736519</v>
+        <v>0.010183278564544943</v>
       </c>
       <c r="H6" t="n">
-        <v>-16.939434352550965</v>
+        <v>-17.27151568455575</v>
       </c>
       <c r="I6" t="n">
         <v>0.0</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.17336780553058911</v>
+        <v>-0.17588065544773837</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.17336780553058911</v>
+        <v>-0.17588065544773837</v>
       </c>
       <c r="L6" t="n">
-        <v>-0.17336780553058911</v>
+        <v>-0.17588065544773837</v>
       </c>
     </row>
     <row r="7">
@@ -422,37 +428,37 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" t="n">
         <v>0.0</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.19067959356666483</v>
+        <v>-0.20186342355980408</v>
       </c>
       <c r="G7" t="n">
-        <v>0.01024631520383841</v>
+        <v>0.01020148842726258</v>
       </c>
       <c r="H7" t="n">
-        <v>-18.609577177094224</v>
+        <v>-19.787644224576276</v>
       </c>
       <c r="I7" t="n">
         <v>0.0</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.19067959356666483</v>
+        <v>-0.20186342355980408</v>
       </c>
       <c r="K7" t="n">
-        <v>-0.19067959356666483</v>
+        <v>-0.20186342355980408</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.19067959356666483</v>
+        <v>-0.20186342355980408</v>
       </c>
     </row>
     <row r="8">
@@ -460,37 +466,37 @@
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="E8" t="n">
         <v>0.0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.6378319308692257</v>
+        <v>-0.17554835007149577</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H8" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I8" t="e">
-        <v>#N/A</v>
+        <v>0.010183062146703406</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-17.239249603158573</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.0</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6378319308692257</v>
+        <v>-0.17554835007149577</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6378319308692257</v>
+        <v>-0.17554835007149577</v>
       </c>
       <c r="L8" t="n">
-        <v>0.6378319308692257</v>
+        <v>-0.17554835007149577</v>
       </c>
     </row>
     <row r="9">
@@ -501,7 +507,7 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -510,7 +516,7 @@
         <v>0.0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.14427243221246433</v>
+        <v>0.6396808147966291</v>
       </c>
       <c r="G9" t="n">
         <v>0.0</v>
@@ -522,13 +528,13 @@
         <v>#N/A</v>
       </c>
       <c r="J9" t="n">
-        <v>0.14427243221246433</v>
+        <v>0.6396808147966291</v>
       </c>
       <c r="K9" t="n">
-        <v>0.14427243221246433</v>
+        <v>0.6396808147966291</v>
       </c>
       <c r="L9" t="n">
-        <v>0.14427243221246433</v>
+        <v>0.6396808147966291</v>
       </c>
     </row>
     <row r="10">
@@ -539,7 +545,7 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>34</v>
@@ -548,7 +554,7 @@
         <v>0.0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.30166862252073756</v>
+        <v>0.14189248421018408</v>
       </c>
       <c r="G10" t="n">
         <v>0.0</v>
@@ -560,13 +566,13 @@
         <v>#N/A</v>
       </c>
       <c r="J10" t="n">
-        <v>0.30166862252073756</v>
+        <v>0.14189248421018408</v>
       </c>
       <c r="K10" t="n">
-        <v>0.30166862252073756</v>
+        <v>0.14189248421018408</v>
       </c>
       <c r="L10" t="n">
-        <v>0.30166862252073756</v>
+        <v>0.14189248421018408</v>
       </c>
     </row>
     <row r="11">
@@ -574,37 +580,37 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E11" t="n">
         <v>0.0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3621680691307743</v>
+        <v>0.3146946745891601</v>
       </c>
       <c r="G11" t="n">
-        <v>0.012258884684045427</v>
-      </c>
-      <c r="H11" t="n">
-        <v>29.543313153285897</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I11" t="e">
+        <v>#N/A</v>
       </c>
       <c r="J11" t="n">
-        <v>0.9999999999999998</v>
+        <v>0.3146946745891601</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9999999999999998</v>
+        <v>0.3146946745891601</v>
       </c>
       <c r="L11" t="n">
-        <v>0.9999999999999998</v>
+        <v>0.3146946745891601</v>
       </c>
     </row>
     <row r="12">
@@ -624,25 +630,25 @@
         <v>0.0</v>
       </c>
       <c r="F12" t="n">
-        <v>1.0</v>
+        <v>0.3603191852033709</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="H12" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I12" t="e">
-        <v>#N/A</v>
+        <v>0.01220740810327819</v>
+      </c>
+      <c r="H12" t="n">
+        <v>29.516436425731555</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.0</v>
       </c>
       <c r="J12" t="n">
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="K12" t="n">
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
       <c r="L12" t="n">
-        <v>1.0</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="13">
@@ -653,7 +659,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -691,7 +697,7 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -726,19 +732,19 @@
         <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E15" t="n">
         <v>0.0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" t="n">
         <v>0.0</v>
@@ -750,13 +756,13 @@
         <v>#N/A</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="K15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -767,10 +773,10 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E16" t="n">
         <v>0.0</v>
@@ -805,10 +811,10 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E17" t="n">
         <v>0.0</v>
@@ -840,13 +846,13 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E18" t="n">
         <v>0.0</v>
@@ -884,16 +890,16 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E19" t="n">
         <v>0.0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.36216806913077426</v>
-      </c>
-      <c r="G19" t="e">
-        <v>#N/A</v>
+        <v>0.0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0</v>
       </c>
       <c r="H19" t="e">
         <v>#N/A</v>
@@ -901,14 +907,14 @@
       <c r="I19" t="e">
         <v>#N/A</v>
       </c>
-      <c r="J19" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K19" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L19" t="e">
-        <v>#N/A</v>
+      <c r="J19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="20">
@@ -919,7 +925,7 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
@@ -928,7 +934,7 @@
         <v>0.0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8557275677875357</v>
+        <v>0.3603191852033709</v>
       </c>
       <c r="G20" t="e">
         <v>#N/A</v>
@@ -957,7 +963,7 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
         <v>34</v>
@@ -966,7 +972,7 @@
         <v>0.0</v>
       </c>
       <c r="F21" t="n">
-        <v>0.6983313774792624</v>
+        <v>0.8581075157898159</v>
       </c>
       <c r="G21" t="e">
         <v>#N/A</v>
@@ -984,6 +990,44 @@
         <v>#N/A</v>
       </c>
       <c r="L21" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.6853053254108399</v>
+      </c>
+      <c r="G22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="I22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K22" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L22" t="e">
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>